<commit_message>
logger correction in timeit
</commit_message>
<xml_diff>
--- a/order_operations/orders.xlsx
+++ b/order_operations/orders.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>gui.yun@e-ports.com</t>
   </si>
@@ -41,22 +41,40 @@
     <t>consigneeName</t>
   </si>
   <si>
+    <t>5a3c970775c03807006362c0</t>
+  </si>
+  <si>
+    <t>EP1120171222052423980</t>
+  </si>
+  <si>
+    <t>5a1bce0899c71b0900f9665a</t>
+  </si>
+  <si>
+    <t>orgOwnerTest.20171117001.a</t>
+  </si>
+  <si>
+    <t>5a1bd30999c71b0900f9665b</t>
+  </si>
+  <si>
+    <t>orgAgentTest.20171127002.b</t>
+  </si>
+  <si>
+    <t>5a3c954d75c03807006362a2</t>
+  </si>
+  <si>
+    <t>EP0620171222051701196</t>
+  </si>
+  <si>
+    <t>5a39cc876556100800cbd47d</t>
+  </si>
+  <si>
+    <t>EP0820171220023551609</t>
+  </si>
+  <si>
     <t>5a2fa92e5e21d70800bc4dc8</t>
   </si>
   <si>
     <t>EP0120171212100222910</t>
-  </si>
-  <si>
-    <t>5a1bce0899c71b0900f9665a</t>
-  </si>
-  <si>
-    <t>orgOwnerTest.20171117001.a</t>
-  </si>
-  <si>
-    <t>5a1bd30999c71b0900f9665b</t>
-  </si>
-  <si>
-    <t>orgAgentTest.20171127002.b</t>
   </si>
   <si>
     <t>5a2f9f0d6f8cd3070026d069</t>
@@ -482,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -655,18 +673,18 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -675,18 +693,18 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -703,22 +721,22 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
+      <c r="F12" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -735,18 +753,18 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -763,10 +781,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -783,21 +801,81 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
         <v>42</v>
       </c>
-      <c r="B16" t="s">
+      <c r="F16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>